<commit_message>
Filling in some gaps in fire-response strategy of taxa using other references besides Nicolle 2006 for species either not mentioned in that census or for which the category has since been determined more robustly.
</commit_message>
<xml_diff>
--- a/Input_data/fire_data.xlsx
+++ b/Input_data/fire_data.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoinettemarieportelli/Dropbox/Eucs Directory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoinettep/Dropbox/Eucs_phylo_traits/Input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9770B8D5-0B32-4A48-87EC-00C0FE5B066B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B84F30-D16E-224B-9D50-C8D279B71217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="460" windowWidth="19960" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="500" windowWidth="20280" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fire.response" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="204">
   <si>
     <t>taxon</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Eucalyptus obliqua</t>
   </si>
   <si>
-    <t>Eucalyptus ovata var. ovata</t>
-  </si>
-  <si>
     <t>Eucalyptus pauciflora subsp. parvifructa</t>
   </si>
   <si>
@@ -463,21 +460,12 @@
     <t>Eucalyptus talyuberlup</t>
   </si>
   <si>
-    <t>Eucalyptus preissiana</t>
-  </si>
-  <si>
     <t>Eucalyptus ligulata subsp. stirlingica</t>
   </si>
   <si>
-    <t>Eucalyptus lehmannii</t>
-  </si>
-  <si>
     <t>Eucalyptus pleurocarpa</t>
   </si>
   <si>
-    <t>Eucalyptus wandoo</t>
-  </si>
-  <si>
     <t>Eucalyptus loxophleba subsp. loxophleba</t>
   </si>
   <si>
@@ -487,18 +475,12 @@
     <t>Eucalyptus incrassata</t>
   </si>
   <si>
-    <t>Eucalyptus decipiens</t>
-  </si>
-  <si>
     <t>Eucalyptus cornuta</t>
   </si>
   <si>
     <t>Eucalyptus angulosa</t>
   </si>
   <si>
-    <t>Eucalyptus thamnoides</t>
-  </si>
-  <si>
     <t>Eucalyptus phaenophylla subsp. phaenophylla</t>
   </si>
   <si>
@@ -508,24 +490,12 @@
     <t>Eucalyptus buprestium</t>
   </si>
   <si>
-    <t>Eucalyptus xanthonema</t>
-  </si>
-  <si>
     <t>Eucalyptus uncinata</t>
   </si>
   <si>
-    <t>Eucalyptus rudis</t>
-  </si>
-  <si>
     <t>Eucalyptus conglobata subsp. perata</t>
   </si>
   <si>
-    <t>Eucalyptus vergrandis</t>
-  </si>
-  <si>
-    <t>Eucalyptus flocktoniae</t>
-  </si>
-  <si>
     <t>Eucalyptus hebetifolia</t>
   </si>
   <si>
@@ -538,9 +508,6 @@
     <t>Eucalyptus megacarpa</t>
   </si>
   <si>
-    <t>Eucalyptus pluricaulis</t>
-  </si>
-  <si>
     <t>using E. beyeri according to Nicolle's idea</t>
   </si>
   <si>
@@ -569,13 +536,131 @@
   </si>
   <si>
     <t>Eucalyptus robusta</t>
+  </si>
+  <si>
+    <t>Corymbia eximia</t>
+  </si>
+  <si>
+    <t>Eucalyptus viridis</t>
+  </si>
+  <si>
+    <t>Sect Adnataria, subsect. Apicales, ser. Buxeales, subser. Continentes</t>
+  </si>
+  <si>
+    <t>Eucalyptus goniocalyx subsp. viridissima</t>
+  </si>
+  <si>
+    <t>Eucalyptus socialis</t>
+  </si>
+  <si>
+    <t>Eucalyptus leucoxylon subsp. pruinosa</t>
+  </si>
+  <si>
+    <t>Same as other subsecies</t>
+  </si>
+  <si>
+    <t>Same as other subspecies</t>
+  </si>
+  <si>
+    <t>Eucalyptus thamnoides subsp. thamnoides</t>
+  </si>
+  <si>
+    <t>Eucalyptus rudis subsp. rudis</t>
+  </si>
+  <si>
+    <t>Eucalyptus preissiana subsp. preissiana</t>
+  </si>
+  <si>
+    <t>Eucalyptus pluricaulis subsp. porphyrea</t>
+  </si>
+  <si>
+    <t>Eucalyptus lehmannii subsp. parallela</t>
+  </si>
+  <si>
+    <t>Eucalyptus flocktoniae subsp. flocktoniae</t>
+  </si>
+  <si>
+    <t>Eucalyptus ovata subsp. ovata</t>
+  </si>
+  <si>
+    <t># No longer needed taxa:</t>
+  </si>
+  <si>
+    <t># Eucalyptus decipiens</t>
+  </si>
+  <si>
+    <t># Note: most taxa do not vary regeneration strategy between subspecies and only one of the above taxa, E. loxophleba is among those that do.</t>
+  </si>
+  <si>
+    <t>Nicolle (2006) says 'unknown' for both possession of lignotuber and sprouting type</t>
+  </si>
+  <si>
+    <t>Neither it or its synonym, E. pyrenea, are in Brooker's treatment, but many of its close relatives are in Brooker's ser. Globulares, subser. Remanentes, which aside from E. nitens and E. denticulata (also in separate series in later tretaments, the rest are combination resprouters</t>
+  </si>
+  <si>
+    <t>Eucalyptus wandoo subsp. wandoo</t>
+  </si>
+  <si>
+    <t>Eucalyptus xanthonema subsp. apposita</t>
+  </si>
+  <si>
+    <t>Eucalyptus vegrandis subsp. vegrandis</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fire response: Resprouts from lignotuber and epicormic buds. Source:Benson, Doug and McDougall, Lyn 1998 Ecology of Sydney plant species: Part 6 Dicotyledon family Myrtaceae </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF211E1E"/>
+        <rFont val="Palatino"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Cunninghamia </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF211E1E"/>
+        <rFont val="Palatino"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">5(4) 808 to 987 </t>
+    </r>
+  </si>
+  <si>
+    <t>Vivian et al 2008 found 2% mortality after severe fire. https://doi.org/10.1111/j.1442-9993.2007.01790.x Nicolle (2006) says no lignotuber and sprouting 'unknown'</t>
+  </si>
+  <si>
+    <t>Nicolle  (2006) says no lignotuber, but sprouting 'unknown'.   Bensobn &amp;Howlell: Fire response: Resprouts from epicormic buds (Fox 1988) after high intensity fire (1/1994)
+at Lane Cove (P. Kubiak pers. comm.).</t>
+  </si>
+  <si>
+    <t>Nicolle  (2006) says no lignotuber, but sprouting 'unknown'. Epicromic sprouter in Vi Fire response database</t>
+  </si>
+  <si>
+    <t>Grant et al 1998 Aust Forestry 60:84-89 presentes data showing epicormic, but not basal resprouting.</t>
+  </si>
+  <si>
+    <t>Grant et al 1998 Aust Forestry 60:84-89 presentes data showing epicormic, but not basal resprouting. Benson &amp; Howell report epicormic srpouting but no basal.</t>
+  </si>
+  <si>
+    <t>Bendal et al https://doi.org/10.1016/j.foreco.2022.120070 mostly epicormic Benson &amp; Howell: Fire response: Resprouts from branches and base after high intensity fire (Bell pers. comm., P. Kubiak pers. comm.).</t>
+  </si>
+  <si>
+    <t>Was stem-only based on Nicolle (2006) explicitly saying it had no lignotuber, but based on Ezra's recent Master's thesis data and the Gill and Moore chapter in Cheney et al. 1992, smaller trees predominantly lignotuber resprout but larger and older ones will mostly epicormically resprout.</t>
+  </si>
+  <si>
+    <t>Note: this subspecies differs in strategy to two of its three sister subspecies, though none of those are inlcuded in this dataset.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -709,6 +794,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF211E1E"/>
+      <name val="Palatino"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF211E1E"/>
+      <name val="Palatino"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1052,8 +1157,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1409,10 +1518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="F170" sqref="F170"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1432,6 +1541,15 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1515,7 +1633,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>186</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -1526,18 +1644,18 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
         <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -1548,7 +1666,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -1559,197 +1677,200 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
         <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
         <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="E17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="E19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
       <c r="F21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="E22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="E23" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="E24" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>33</v>
       </c>
-      <c r="E25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="E26" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>35</v>
       </c>
-      <c r="E27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>36</v>
       </c>
-      <c r="E28" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>37</v>
       </c>
-      <c r="E29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="E30" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>39</v>
-      </c>
-      <c r="E31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>40</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -1760,51 +1881,51 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E33" t="s">
         <v>5</v>
       </c>
       <c r="F33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E34" t="s">
         <v>5</v>
       </c>
       <c r="F34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E35" t="s">
         <v>5</v>
       </c>
       <c r="F35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
         <v>5</v>
       </c>
       <c r="F36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" t="s">
         <v>5</v>
@@ -1815,7 +1936,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E38" t="s">
         <v>5</v>
@@ -1826,7 +1947,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" t="s">
         <v>5</v>
@@ -1837,7 +1958,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" t="s">
         <v>5</v>
@@ -1848,7 +1969,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E41" t="s">
         <v>5</v>
@@ -1859,7 +1980,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E42" t="s">
         <v>5</v>
@@ -1870,7 +1991,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
         <v>5</v>
@@ -1881,21 +2002,21 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" t="s">
         <v>52</v>
-      </c>
-      <c r="E44" t="s">
-        <v>5</v>
-      </c>
-      <c r="F44" t="s">
-        <v>6</v>
-      </c>
-      <c r="G44" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E45" t="s">
         <v>5</v>
@@ -1906,7 +2027,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E46" t="s">
         <v>5</v>
@@ -1917,12 +2038,21 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="E47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E48" t="s">
         <v>5</v>
@@ -1933,7 +2063,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E49" t="s">
         <v>5</v>
@@ -1944,51 +2074,60 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E50" t="s">
         <v>5</v>
       </c>
       <c r="F50" t="s">
-        <v>174</v>
+        <v>16</v>
+      </c>
+      <c r="G50" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E51" t="s">
         <v>5</v>
       </c>
       <c r="F51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E52" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="F52" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="G52" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E53" t="s">
         <v>5</v>
       </c>
       <c r="F53" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="G53" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E54" t="s">
         <v>5</v>
@@ -1997,12 +2136,12 @@
         <v>6</v>
       </c>
       <c r="G54" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E55" t="s">
         <v>5</v>
@@ -2013,7 +2152,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E56" t="s">
         <v>5</v>
@@ -2024,7 +2163,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E57" t="s">
         <v>5</v>
@@ -2035,7 +2174,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E58" t="s">
         <v>5</v>
@@ -2046,7 +2185,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E59" t="s">
         <v>5</v>
@@ -2057,7 +2196,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E60" t="s">
         <v>5</v>
@@ -2068,7 +2207,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E61" t="s">
         <v>5</v>
@@ -2079,7 +2218,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E62" t="s">
         <v>5</v>
@@ -2090,386 +2229,401 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="E63" t="s">
+        <v>22</v>
+      </c>
+      <c r="F63" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>72</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>73</v>
       </c>
-      <c r="E64" t="s">
-        <v>5</v>
-      </c>
-      <c r="F64" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="E65" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>74</v>
       </c>
-      <c r="E65" t="s">
-        <v>5</v>
-      </c>
-      <c r="F65" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="E66" t="s">
         <v>75</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>76</v>
       </c>
-      <c r="F66" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="E67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>77</v>
       </c>
-      <c r="E67" t="s">
-        <v>5</v>
-      </c>
-      <c r="F67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="E68" t="s">
+        <v>5</v>
+      </c>
+      <c r="F68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>78</v>
       </c>
-      <c r="E68" t="s">
-        <v>5</v>
-      </c>
-      <c r="F68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="E69" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>79</v>
       </c>
-      <c r="E69" t="s">
-        <v>5</v>
-      </c>
-      <c r="F69" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="E70" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" t="s">
+        <v>163</v>
+      </c>
+      <c r="G70" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>80</v>
       </c>
-      <c r="E70" t="s">
-        <v>5</v>
-      </c>
-      <c r="F70" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="E71" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>81</v>
       </c>
-      <c r="E71" t="s">
-        <v>5</v>
-      </c>
-      <c r="F71" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="E72" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>82</v>
       </c>
-      <c r="E72" t="s">
-        <v>5</v>
-      </c>
-      <c r="F72" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="E73" t="s">
+        <v>5</v>
+      </c>
+      <c r="F73" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>83</v>
       </c>
-      <c r="E73" t="s">
-        <v>5</v>
-      </c>
-      <c r="F73" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="E74" t="s">
+        <v>5</v>
+      </c>
+      <c r="F74" t="s">
+        <v>163</v>
+      </c>
+      <c r="G74" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>84</v>
       </c>
-      <c r="E74" t="s">
-        <v>23</v>
-      </c>
-      <c r="F74" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="E75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>85</v>
       </c>
-      <c r="E75" t="s">
-        <v>5</v>
-      </c>
-      <c r="F75" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="E76" t="s">
+        <v>5</v>
+      </c>
+      <c r="F76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>86</v>
       </c>
-      <c r="E76" t="s">
-        <v>5</v>
-      </c>
-      <c r="F76" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="E77" t="s">
+        <v>5</v>
+      </c>
+      <c r="F77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>87</v>
       </c>
-      <c r="E77" t="s">
-        <v>5</v>
-      </c>
-      <c r="F77" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="E78" t="s">
+        <v>5</v>
+      </c>
+      <c r="F78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>88</v>
       </c>
-      <c r="E78" t="s">
-        <v>5</v>
-      </c>
-      <c r="F78" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="E79" t="s">
+        <v>75</v>
+      </c>
+      <c r="F79" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>89</v>
       </c>
-      <c r="E79" t="s">
-        <v>76</v>
-      </c>
-      <c r="F79" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="E80" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>90</v>
       </c>
-      <c r="E80" t="s">
-        <v>5</v>
-      </c>
-      <c r="F80" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="E81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>91</v>
       </c>
-      <c r="E81" t="s">
-        <v>5</v>
-      </c>
-      <c r="F81" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="E82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>92</v>
       </c>
-      <c r="E82" t="s">
-        <v>5</v>
-      </c>
-      <c r="F82" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="E83" t="s">
+        <v>5</v>
+      </c>
+      <c r="F83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>93</v>
       </c>
-      <c r="E83" t="s">
-        <v>5</v>
-      </c>
-      <c r="F83" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="E84" t="s">
+        <v>5</v>
+      </c>
+      <c r="F84" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>94</v>
       </c>
-      <c r="E84" t="s">
-        <v>5</v>
-      </c>
-      <c r="F84" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="E85" t="s">
+        <v>5</v>
+      </c>
+      <c r="F85" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>95</v>
       </c>
-      <c r="E85" t="s">
-        <v>5</v>
-      </c>
-      <c r="F85" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="E86" t="s">
+        <v>5</v>
+      </c>
+      <c r="F86" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>96</v>
       </c>
-      <c r="E86" t="s">
-        <v>5</v>
-      </c>
-      <c r="F86" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="E87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>97</v>
       </c>
-      <c r="E87" t="s">
-        <v>5</v>
-      </c>
-      <c r="F87" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="E88" t="s">
+        <v>5</v>
+      </c>
+      <c r="F88" t="s">
+        <v>163</v>
+      </c>
+      <c r="G88" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>98</v>
       </c>
-      <c r="E88" t="s">
-        <v>23</v>
-      </c>
-      <c r="F88" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="E89" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>99</v>
       </c>
-      <c r="E89" t="s">
-        <v>5</v>
-      </c>
-      <c r="F89" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="E90" t="s">
+        <v>5</v>
+      </c>
+      <c r="F90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>100</v>
       </c>
-      <c r="E90" t="s">
-        <v>5</v>
-      </c>
-      <c r="F90" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="E91" t="s">
+        <v>5</v>
+      </c>
+      <c r="F91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>101</v>
       </c>
-      <c r="E91" t="s">
-        <v>5</v>
-      </c>
-      <c r="F91" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="E92" t="s">
+        <v>5</v>
+      </c>
+      <c r="F92" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>102</v>
       </c>
-      <c r="E92" t="s">
-        <v>5</v>
-      </c>
-      <c r="F92" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="E93" t="s">
+        <v>75</v>
+      </c>
+      <c r="F93" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>103</v>
       </c>
-      <c r="E93" t="s">
-        <v>76</v>
-      </c>
-      <c r="F93" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="E94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>104</v>
       </c>
-      <c r="E94" t="s">
-        <v>5</v>
-      </c>
-      <c r="F94" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="E95" t="s">
+        <v>5</v>
+      </c>
+      <c r="F95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>105</v>
       </c>
-      <c r="E95" t="s">
-        <v>5</v>
-      </c>
-      <c r="F95" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>106</v>
-      </c>
       <c r="E96" t="s">
         <v>5</v>
       </c>
       <c r="F96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E97" t="s">
         <v>5</v>
       </c>
       <c r="F97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E98" t="s">
         <v>5</v>
@@ -2480,7 +2634,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E99" t="s">
         <v>5</v>
@@ -2491,7 +2645,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E100" t="s">
         <v>5</v>
@@ -2502,7 +2656,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E101" t="s">
         <v>5</v>
@@ -2513,7 +2667,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E102" t="s">
         <v>5</v>
@@ -2524,7 +2678,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E103" t="s">
         <v>5</v>
@@ -2535,7 +2689,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E104" t="s">
         <v>5</v>
@@ -2546,7 +2700,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E105" t="s">
         <v>5</v>
@@ -2557,7 +2711,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E106" t="s">
         <v>5</v>
@@ -2568,7 +2722,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E107" t="s">
         <v>5</v>
@@ -2579,7 +2733,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E108" t="s">
         <v>5</v>
@@ -2590,7 +2744,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E109" t="s">
         <v>5</v>
@@ -2601,7 +2755,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E110" t="s">
         <v>5</v>
@@ -2612,7 +2766,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E111" t="s">
         <v>5</v>
@@ -2623,7 +2777,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E112" t="s">
         <v>5</v>
@@ -2634,7 +2788,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E113" t="s">
         <v>5</v>
@@ -2645,18 +2799,18 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E114" t="s">
         <v>5</v>
       </c>
       <c r="F114" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E115" t="s">
         <v>5</v>
@@ -2667,32 +2821,32 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>125</v>
+      </c>
+      <c r="E116" t="s">
+        <v>5</v>
+      </c>
+      <c r="F116" t="s">
+        <v>6</v>
+      </c>
+      <c r="G116" t="s">
         <v>126</v>
-      </c>
-      <c r="E116" t="s">
-        <v>5</v>
-      </c>
-      <c r="F116" t="s">
-        <v>6</v>
-      </c>
-      <c r="G116" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E117" t="s">
         <v>5</v>
       </c>
       <c r="F117" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E118" t="s">
         <v>5</v>
@@ -2703,7 +2857,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E119" t="s">
         <v>5</v>
@@ -2714,21 +2868,21 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>130</v>
+      </c>
+      <c r="E120" t="s">
+        <v>22</v>
+      </c>
+      <c r="F120" t="s">
+        <v>22</v>
+      </c>
+      <c r="G120" t="s">
         <v>131</v>
-      </c>
-      <c r="E120" t="s">
-        <v>23</v>
-      </c>
-      <c r="F120" t="s">
-        <v>23</v>
-      </c>
-      <c r="G120" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E121" t="s">
         <v>5</v>
@@ -2739,29 +2893,29 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E122" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F122" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E123" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F123" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E124" t="s">
         <v>5</v>
@@ -2772,7 +2926,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E125" t="s">
         <v>5</v>
@@ -2783,7 +2937,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E126" t="s">
         <v>5</v>
@@ -2794,392 +2948,398 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>138</v>
+      </c>
+      <c r="E127" t="s">
+        <v>5</v>
+      </c>
+      <c r="F127" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>139</v>
       </c>
-      <c r="E127" t="s">
-        <v>5</v>
-      </c>
-      <c r="F127" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+      <c r="E129" t="s">
+        <v>5</v>
+      </c>
+      <c r="F129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>140</v>
       </c>
-      <c r="E129" t="s">
-        <v>5</v>
-      </c>
-      <c r="F129" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+      <c r="E130" t="s">
+        <v>5</v>
+      </c>
+      <c r="F130" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>141</v>
       </c>
-      <c r="E130" t="s">
-        <v>5</v>
-      </c>
-      <c r="F130" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="E131" t="s">
+        <v>5</v>
+      </c>
+      <c r="F131" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>142</v>
       </c>
-      <c r="E131" t="s">
-        <v>5</v>
-      </c>
-      <c r="F131" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="E132" t="s">
+        <v>5</v>
+      </c>
+      <c r="F132" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>143</v>
       </c>
-      <c r="E132" t="s">
-        <v>5</v>
-      </c>
-      <c r="F132" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+      <c r="E133" t="s">
+        <v>5</v>
+      </c>
+      <c r="F133" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>144</v>
       </c>
-      <c r="E133" t="s">
-        <v>5</v>
-      </c>
-      <c r="F133" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+      <c r="E134" t="s">
+        <v>5</v>
+      </c>
+      <c r="F134" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>145</v>
       </c>
-      <c r="E134" t="s">
-        <v>5</v>
-      </c>
-      <c r="F134" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="E135" t="s">
+        <v>5</v>
+      </c>
+      <c r="F135" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>182</v>
+      </c>
+      <c r="E136" t="s">
+        <v>5</v>
+      </c>
+      <c r="F136" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
         <v>146</v>
       </c>
-      <c r="E135" t="s">
-        <v>5</v>
-      </c>
-      <c r="F135" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+      <c r="E137" t="s">
+        <v>5</v>
+      </c>
+      <c r="F137" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>184</v>
+      </c>
+      <c r="E138" t="s">
+        <v>5</v>
+      </c>
+      <c r="F138" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>147</v>
       </c>
-      <c r="E136" t="s">
-        <v>5</v>
-      </c>
-      <c r="F136" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
+      <c r="E139" t="s">
+        <v>5</v>
+      </c>
+      <c r="F139" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>192</v>
+      </c>
+      <c r="E140" t="s">
+        <v>5</v>
+      </c>
+      <c r="F140" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>148</v>
       </c>
-      <c r="E137" t="s">
-        <v>5</v>
-      </c>
-      <c r="F137" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+      <c r="E141" t="s">
+        <v>5</v>
+      </c>
+      <c r="F141" t="s">
+        <v>6</v>
+      </c>
+      <c r="G141" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>149</v>
       </c>
-      <c r="E138" t="s">
-        <v>5</v>
-      </c>
-      <c r="F138" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
+      <c r="E142" t="s">
+        <v>5</v>
+      </c>
+      <c r="F142" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>150</v>
       </c>
-      <c r="E139" t="s">
-        <v>5</v>
-      </c>
-      <c r="F139" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
+      <c r="E143" t="s">
+        <v>5</v>
+      </c>
+      <c r="F143" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
         <v>151</v>
       </c>
-      <c r="E140" t="s">
-        <v>5</v>
-      </c>
-      <c r="F140" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+      <c r="E144" t="s">
+        <v>5</v>
+      </c>
+      <c r="F144" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>152</v>
       </c>
-      <c r="E141" t="s">
-        <v>5</v>
-      </c>
-      <c r="F141" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+      <c r="E145" t="s">
+        <v>5</v>
+      </c>
+      <c r="F145" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>180</v>
+      </c>
+      <c r="E146" t="s">
+        <v>5</v>
+      </c>
+      <c r="F146" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>153</v>
       </c>
-      <c r="E142" t="s">
-        <v>5</v>
-      </c>
-      <c r="F142" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+      <c r="E147" t="s">
+        <v>5</v>
+      </c>
+      <c r="F147" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>154</v>
       </c>
-      <c r="E143" t="s">
-        <v>5</v>
-      </c>
-      <c r="F143" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+      <c r="E148" t="s">
+        <v>5</v>
+      </c>
+      <c r="F148" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>155</v>
       </c>
-      <c r="E144" t="s">
-        <v>5</v>
-      </c>
-      <c r="F144" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+      <c r="E149" t="s">
+        <v>5</v>
+      </c>
+      <c r="F149" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>193</v>
+      </c>
+      <c r="E150" t="s">
+        <v>5</v>
+      </c>
+      <c r="F150" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>156</v>
       </c>
-      <c r="E145" t="s">
-        <v>5</v>
-      </c>
-      <c r="F145" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+      <c r="E151" t="s">
+        <v>5</v>
+      </c>
+      <c r="F151" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>181</v>
+      </c>
+      <c r="E152" t="s">
+        <v>5</v>
+      </c>
+      <c r="F152" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>157</v>
       </c>
-      <c r="E146" t="s">
-        <v>5</v>
-      </c>
-      <c r="F146" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+      <c r="E153" t="s">
+        <v>5</v>
+      </c>
+      <c r="F153" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>194</v>
+      </c>
+      <c r="E154" t="s">
+        <v>5</v>
+      </c>
+      <c r="F154" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>185</v>
+      </c>
+      <c r="E155" t="s">
+        <v>5</v>
+      </c>
+      <c r="F155" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>158</v>
       </c>
-      <c r="E147" t="s">
-        <v>5</v>
-      </c>
-      <c r="F147" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="E156" t="s">
+        <v>5</v>
+      </c>
+      <c r="F156" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>159</v>
       </c>
-      <c r="E148" t="s">
-        <v>5</v>
-      </c>
-      <c r="F148" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="E157" t="s">
+        <v>5</v>
+      </c>
+      <c r="F157" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>160</v>
       </c>
-      <c r="E149" t="s">
-        <v>5</v>
-      </c>
-      <c r="F149" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="E158" t="s">
+        <v>5</v>
+      </c>
+      <c r="F158" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>161</v>
       </c>
-      <c r="E150" t="s">
-        <v>5</v>
-      </c>
-      <c r="F150" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>162</v>
-      </c>
-      <c r="E151" t="s">
-        <v>5</v>
-      </c>
-      <c r="F151" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+      <c r="E159" t="s">
+        <v>5</v>
+      </c>
+      <c r="F159" t="s">
         <v>163</v>
       </c>
-      <c r="E152" t="s">
-        <v>5</v>
-      </c>
-      <c r="F152" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
-        <v>164</v>
-      </c>
-      <c r="E153" t="s">
-        <v>5</v>
-      </c>
-      <c r="F153" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
-        <v>165</v>
-      </c>
-      <c r="E154" t="s">
-        <v>5</v>
-      </c>
-      <c r="F154" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>166</v>
-      </c>
-      <c r="E155" t="s">
-        <v>5</v>
-      </c>
-      <c r="F155" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>167</v>
-      </c>
-      <c r="E156" t="s">
-        <v>5</v>
-      </c>
-      <c r="F156" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
-        <v>168</v>
-      </c>
-      <c r="E157" t="s">
-        <v>5</v>
-      </c>
-      <c r="F157" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>169</v>
-      </c>
-      <c r="E158" t="s">
-        <v>5</v>
-      </c>
-      <c r="F158" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>170</v>
-      </c>
-      <c r="E159" t="s">
-        <v>5</v>
-      </c>
-      <c r="F159" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G159" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="E160" t="s">
         <v>5</v>
       </c>
       <c r="F160" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E161" t="s">
         <v>5</v>
       </c>
       <c r="F161" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="E162" t="s">
         <v>5</v>
       </c>
       <c r="F162" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E163" t="s">
         <v>5</v>
@@ -3190,7 +3350,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="E164" t="s">
         <v>5</v>
@@ -3201,49 +3361,126 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E165" t="s">
         <v>5</v>
       </c>
       <c r="F165" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="G165" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E166" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="F166" t="s">
-        <v>29</v>
-      </c>
-      <c r="G166" t="s">
-        <v>180</v>
+        <v>75</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E167" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="F167" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E168" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="F168" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>173</v>
+      </c>
+      <c r="E169" t="s">
+        <v>5</v>
+      </c>
+      <c r="F169" t="s">
+        <v>28</v>
+      </c>
+      <c r="G169" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>175</v>
+      </c>
+      <c r="E170" t="s">
+        <v>5</v>
+      </c>
+      <c r="F170" t="s">
+        <v>6</v>
+      </c>
+      <c r="G170" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>177</v>
+      </c>
+      <c r="E171" t="s">
+        <v>5</v>
+      </c>
+      <c r="F171" t="s">
+        <v>6</v>
+      </c>
+      <c r="G171" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>176</v>
+      </c>
+      <c r="E172" t="s">
+        <v>5</v>
+      </c>
+      <c r="F172" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>